<commit_message>
added open search url entering
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>But if the JQM is upgraded the dismissable property is added so it can be used-to be decided</t>
+  </si>
+  <si>
+    <t>open search url for search</t>
+  </si>
+  <si>
+    <t>According to specs the user has the possibility to enter his own open search url. For the moment it is not possible</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,6 +501,20 @@
       </c>
       <c r="D5" s="2"/>
     </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added assignee column add download options issue
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>According to specs the user has the possibility to enter his own open search url. For the moment it is not possible</t>
+  </si>
+  <si>
+    <t>The selected download options are not set when opening the STO widget</t>
+  </si>
+  <si>
+    <t>selected download options</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>EM</t>
   </si>
 </sst>
 </file>
@@ -110,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +132,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +452,7 @@
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +465,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -464,8 +482,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -478,8 +499,11 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -492,16 +516,22 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -513,6 +543,26 @@
       </c>
       <c r="D6" t="s">
         <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added map display issue
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>The timebox/datebox plugin does not allow seconds choice. However, the seconds are added by the client to be 00. For the moment, we have decided to use the plugin as it is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2D mode, the map can be dragged untill seeing the eadges of the map </t>
+  </si>
+  <si>
+    <t>map display</t>
   </si>
 </sst>
 </file>
@@ -445,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,8 +592,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed seconds handling in search widgets (ngeo 366)
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -73,12 +73,6 @@
   </si>
   <si>
     <t>EM</t>
-  </si>
-  <si>
-    <t>seconds handling in dates widgets</t>
-  </si>
-  <si>
-    <t>The timebox/datebox plugin does not allow seconds choice. However, the seconds are added by the client to be 00. For the moment, we have decided to use the plugin as it is.</t>
   </si>
   <si>
     <t xml:space="preserve">In 2D mode, the map can be dragged untill seeing the eadges of the map </t>
@@ -449,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,31 +572,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documentation for CDR delivery.
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>map display</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>An error message should be displayed when the server does not answer, or does not answer correctly</t>
   </si>
 </sst>
 </file>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +592,20 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated with the done tasks
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -51,15 +51,6 @@
     <t xml:space="preserve">Change the headers to be in the top of the widget rather inside the widget content. </t>
   </si>
   <si>
-    <t>not use jqm popups but a custom component to allow closing the widget.</t>
-  </si>
-  <si>
-    <t>But if the JQM is upgraded the dismissable property is added so it can be used-to be decided</t>
-  </si>
-  <si>
-    <t>open search url for search</t>
-  </si>
-  <si>
     <t>According to specs the user has the possibility to enter his own open search url. For the moment it is not possible</t>
   </si>
   <si>
@@ -88,6 +79,18 @@
   </si>
   <si>
     <t>An error message should be displayed when the server does not answer, or does not answer correctly</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>not use jqm popups but a custom component to allow closing the widget.But if the JQM is upgraded the dismissable property is added so it can be used-to be decided</t>
+  </si>
+  <si>
+    <t>Enter openSearch url for search</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5AC664"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,7 +157,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -157,6 +174,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5AC664"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,13 +474,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" customWidth="1"/>
@@ -481,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -499,114 +521,109 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +638,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -633,7 +650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update error message handling
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,7 +157,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -477,7 +476,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,36 +524,36 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -576,53 +575,53 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documentation for validation
</commit_message>
<xml_diff>
--- a/documentation/ngEO-WEBC-internal-issues.xlsx
+++ b/documentation/ngEO-WEBC-internal-issues.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Sprint NB</t>
   </si>
@@ -91,6 +91,33 @@
   </si>
   <si>
     <t>Enter openSearch url for search</t>
+  </si>
+  <si>
+    <t>CDR</t>
+  </si>
+  <si>
+    <t>Product Download</t>
+  </si>
+  <si>
+    <t>Browse URL</t>
+  </si>
+  <si>
+    <t>What we should expect ?</t>
+  </si>
+  <si>
+    <t>Name/Description in DataSet Selection</t>
+  </si>
+  <si>
+    <t>Paging issue</t>
+  </si>
+  <si>
+    <t>Automatic ? Manual ?</t>
+  </si>
+  <si>
+    <t>Granule representation in the Web Client</t>
+  </si>
+  <si>
+    <t>Diffenriate between Direct Download and Download with Local DM</t>
   </si>
 </sst>
 </file>
@@ -187,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -473,16 +500,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -558,20 +585,20 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="E5" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -623,6 +650,70 @@
       </c>
       <c r="E8" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +728,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -649,7 +740,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>